<commit_message>
Major Refactor to add categories to operators. Used the time to convert to new-style constructor to create builtin operators. Added more unit tests to verify changes.
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/xls/sampleMath.xlsx
+++ b/test/src/org/tms/io/xls/sampleMath.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19780" yWindow="20" windowWidth="18880" windowHeight="9980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,22 @@
     <definedName name="ASinVal">Sheet1!$B$11</definedName>
     <definedName name="ATanDVal">Sheet1!$B$14</definedName>
     <definedName name="ATanVal">Sheet1!$B$13</definedName>
-    <definedName name="CombinVal">Sheet1!$D$10</definedName>
+    <definedName name="CeilVal">Sheet1!$D$9</definedName>
+    <definedName name="CombinVal">Sheet1!$D$11</definedName>
     <definedName name="CosHVal">Sheet1!$B$21</definedName>
     <definedName name="CosVal">Sheet1!$B$16</definedName>
     <definedName name="ExpVal">Sheet1!$D$2</definedName>
-    <definedName name="GcdVal">Sheet1!$D$13</definedName>
+    <definedName name="FACT">Sheet1!$C$17</definedName>
+    <definedName name="FactVal">Sheet1!$D$17</definedName>
+    <definedName name="GcdVal">Sheet1!$D$14</definedName>
     <definedName name="IntVal">Sheet1!$D$7</definedName>
-    <definedName name="LcmVal">Sheet1!$D$14</definedName>
+    <definedName name="LcmVal">Sheet1!$D$15</definedName>
     <definedName name="LnVal">Sheet1!$D$3</definedName>
     <definedName name="Log10Val">Sheet1!$D$4</definedName>
     <definedName name="LogVal">Sheet1!$D$5</definedName>
-    <definedName name="PermutVal">Sheet1!$D$11</definedName>
+    <definedName name="ModVal">Sheet1!$D$19</definedName>
+    <definedName name="PermutVal">Sheet1!$D$12</definedName>
+    <definedName name="PiVal">Sheet1!$D$18</definedName>
     <definedName name="RandBetweenVal">Sheet1!$B$3</definedName>
     <definedName name="RandVal">Sheet1!$B$2</definedName>
     <definedName name="SignVal">Sheet1!$B$7</definedName>
@@ -48,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -135,6 +140,18 @@
   </si>
   <si>
     <t>LCM</t>
+  </si>
+  <si>
+    <t>CEIL</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>MOD</t>
+  </si>
+  <si>
+    <t>FACT</t>
   </si>
 </sst>
 </file>
@@ -581,13 +598,14 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
     <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -610,7 +628,7 @@
       </c>
       <c r="B2">
         <f ca="1">RAND()</f>
-        <v>0.27597019537165068</v>
+        <v>0.30716686874024357</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -703,6 +721,13 @@
         <f>ACOS(-0.5)</f>
         <v>2.0943951023931957</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <f>CEILING(18.7, 1)</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
@@ -712,13 +737,6 @@
         <f>DEGREES(ACOS(-0.5))</f>
         <v>120.00000000000001</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <f>COMBIN(6,3)</f>
-        <v>20</v>
-      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
@@ -729,11 +747,11 @@
         <v>0.52359877559829893</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <f>PERMUT(6,3)</f>
-        <v>120</v>
+        <f>COMBIN(6,3)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -744,6 +762,13 @@
         <f>DEGREES(ASIN(0.5))</f>
         <v>30.000000000000004</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12">
+        <f>PERMUT(6,3)</f>
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
@@ -753,13 +778,6 @@
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13">
-        <f>GCD(56, 21)</f>
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
@@ -770,9 +788,18 @@
         <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <f>GCD(56, 21)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f>LCM(24, 36)</f>
         <v>72</v>
       </c>
@@ -786,7 +813,7 @@
         <v>-0.50000000000000022</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -794,8 +821,15 @@
         <f>SIN(ASinVal)</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <f>FACT(6)</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -803,8 +837,24 @@
         <f>TAN(ATanVal)</f>
         <v>0.99999999999999989</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <f>MOD(5,3)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -813,7 +863,7 @@
         <v>1.1752011936438014</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -822,7 +872,7 @@
         <v>1.5430806348152437</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Added more unit tests for basic functions
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/xls/sampleMath.xlsx
+++ b/test/src/org/tms/io/xls/sampleMath.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1520" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <definedName name="ExpVal">Sheet1!$D$2</definedName>
     <definedName name="FACT">Sheet1!$C$17</definedName>
     <definedName name="FactVal">Sheet1!$D$17</definedName>
+    <definedName name="FalseVal">Sheet1!$F$9</definedName>
     <definedName name="GcdVal">Sheet1!$D$14</definedName>
+    <definedName name="IfElseVal">Sheet1!$F$11</definedName>
+    <definedName name="IfVal">Sheet1!$F$10</definedName>
     <definedName name="IntVal">Sheet1!$D$7</definedName>
     <definedName name="LcmVal">Sheet1!$D$15</definedName>
     <definedName name="LnVal">Sheet1!$D$3</definedName>
@@ -33,14 +36,21 @@
     <definedName name="ModVal">Sheet1!$D$19</definedName>
     <definedName name="PermutVal">Sheet1!$D$12</definedName>
     <definedName name="PiVal">Sheet1!$D$18</definedName>
+    <definedName name="PowOpVal">Sheet1!$D$20</definedName>
+    <definedName name="PowVal">Sheet1!$D$21</definedName>
+    <definedName name="QuoVal">Sheet1!$F$5</definedName>
     <definedName name="RandBetweenVal">Sheet1!$B$3</definedName>
     <definedName name="RandVal">Sheet1!$B$2</definedName>
+    <definedName name="RoundVal">Sheet1!$F$6</definedName>
     <definedName name="SignVal">Sheet1!$B$7</definedName>
     <definedName name="SinHVal">Sheet1!$B$20</definedName>
     <definedName name="SinVal">Sheet1!$B$17</definedName>
     <definedName name="SqrtVal">Sheet1!$B$6</definedName>
     <definedName name="TanHVal">Sheet1!$B$22</definedName>
     <definedName name="TanVal">Sheet1!$B$18</definedName>
+    <definedName name="ToDegVal">Sheet1!$F$2</definedName>
+    <definedName name="ToRadVal">Sheet1!$F$3</definedName>
+    <definedName name="TrueVal">Sheet1!$F$8</definedName>
     <definedName name="TruncVal">Sheet1!$D$8</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -53,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +162,30 @@
   </si>
   <si>
     <t>FACT</t>
+  </si>
+  <si>
+    <t>POW ^</t>
+  </si>
+  <si>
+    <t>POW</t>
+  </si>
+  <si>
+    <t>TO DEG</t>
+  </si>
+  <si>
+    <t>TO RAD</t>
+  </si>
+  <si>
+    <t>QUOTIENT</t>
+  </si>
+  <si>
+    <t>ROUND</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>IF ELSE</t>
   </si>
 </sst>
 </file>
@@ -595,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -608,7 +642,7 @@
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -621,14 +655,20 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <f ca="1">RAND()</f>
-        <v>0.30716686874024357</v>
+        <v>0.72853106758204589</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -637,14 +677,21 @@
         <f>EXP(1)</f>
         <v>2.7182818284590451</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <f>DEGREES(PI()/2)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(-5,20)</f>
-        <v>12</v>
+        <v>-2</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -653,8 +700,15 @@
         <f>LN(ExpVal)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <f>RADIANS(90)</f>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
@@ -662,8 +716,9 @@
         <f>LOG10(100)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -678,8 +733,15 @@
         <f>LOG(10)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5">
+        <f>QUOTIENT(7, 2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -687,8 +749,15 @@
         <f>SQRT(64)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <f>ROUND(18.7, 0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -703,8 +772,9 @@
         <f>INT(18.7)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
@@ -712,8 +782,15 @@
         <f>TRUNC(18.7)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -728,8 +805,15 @@
         <f>CEILING(18.7, 1)</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -737,8 +821,15 @@
         <f>DEGREES(ACOS(-0.5))</f>
         <v>120.00000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10">
+        <f>IF(AbsVal &gt; 4, 3, 1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -753,8 +844,15 @@
         <f>COMBIN(6,3)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <f>IF(AbsVal &lt; 4, 3, 1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -769,8 +867,9 @@
         <f>PERMUT(6,3)</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -778,8 +877,9 @@
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -794,8 +894,9 @@
         <f>GCD(56, 21)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
@@ -803,8 +904,9 @@
         <f>LCM(24, 36)</f>
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -812,8 +914,9 @@
         <f>COS(ACosVal)</f>
         <v>-0.50000000000000022</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -828,8 +931,9 @@
         <f>FACT(6)</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -844,8 +948,9 @@
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5">
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
@@ -853,8 +958,9 @@
         <f>MOD(5,3)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
@@ -862,8 +968,16 @@
         <f>SINH(1)</f>
         <v>1.1752011936438014</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <f>2^3</f>
+        <v>8</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -871,8 +985,16 @@
         <f>COSH(1)</f>
         <v>1.5430806348152437</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21">
+        <f>POWER(2, 3)</f>
+        <v>8</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -880,6 +1002,13 @@
         <f>TANH(1)</f>
         <v>0.76159415595576485</v>
       </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="E24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Implemented toEven and toOdd operators
</commit_message>
<xml_diff>
--- a/test/src/org/tms/io/xls/sampleMath.xlsx
+++ b/test/src/org/tms/io/xls/sampleMath.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="860" yWindow="220" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <definedName name="CombinVal">Sheet1!$D$11</definedName>
     <definedName name="CosHVal">Sheet1!$B$21</definedName>
     <definedName name="CosVal">Sheet1!$B$16</definedName>
+    <definedName name="EvenNegVal">Sheet1!$F$14</definedName>
+    <definedName name="EvenVal">Sheet1!$F$13</definedName>
     <definedName name="ExpVal">Sheet1!$D$2</definedName>
     <definedName name="FACT">Sheet1!$C$17</definedName>
     <definedName name="FactVal">Sheet1!$D$17</definedName>
@@ -34,6 +36,8 @@
     <definedName name="Log10Val">Sheet1!$D$4</definedName>
     <definedName name="LogVal">Sheet1!$D$5</definedName>
     <definedName name="ModVal">Sheet1!$D$19</definedName>
+    <definedName name="OddNegVal">Sheet1!$F$16</definedName>
+    <definedName name="OddVal">Sheet1!$F$15</definedName>
     <definedName name="PermutVal">Sheet1!$D$12</definedName>
     <definedName name="PiVal">Sheet1!$D$18</definedName>
     <definedName name="PowOpVal">Sheet1!$D$20</definedName>
@@ -63,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -186,6 +190,18 @@
   </si>
   <si>
     <t>IF ELSE</t>
+  </si>
+  <si>
+    <t>EVEN</t>
+  </si>
+  <si>
+    <t>EVEN -</t>
+  </si>
+  <si>
+    <t>ODD</t>
+  </si>
+  <si>
+    <t>ODD -</t>
   </si>
 </sst>
 </file>
@@ -631,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -668,7 +684,7 @@
       </c>
       <c r="B2">
         <f ca="1">RAND()</f>
-        <v>0.72853106758204589</v>
+        <v>4.2319884396166407E-2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -691,7 +707,7 @@
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(-5,20)</f>
-        <v>-2</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -877,7 +893,13 @@
         <f>ATAN(1)</f>
         <v>0.78539816339744828</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13">
+        <f>EVEN(2.91)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
@@ -894,7 +916,13 @@
         <f>GCD(56, 21)</f>
         <v>7</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14">
+        <f>EVEN(-7.8)</f>
+        <v>-8</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="2" t="s">
@@ -904,7 +932,13 @@
         <f>LCM(24, 36)</f>
         <v>72</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15">
+        <f>ODD(2.91)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
@@ -914,7 +948,13 @@
         <f>COS(ACosVal)</f>
         <v>-0.50000000000000022</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16">
+        <f>ODD(-7.8)</f>
+        <v>-9</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">

</xml_diff>